<commit_message>
FE: Updates for free-sample-rfp and thanks-for-download-free-sample-rfp pages.
</commit_message>
<xml_diff>
--- a/pages/assets/files/ecommerce-sample-rfp-template-by-virto.xlsx
+++ b/pages/assets/files/ecommerce-sample-rfp-template-by-virto.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://virto365.sharepoint.com/sites/VirtoCommerce/Shared Documents/Marketing/Messaging &amp; Content/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/meganpennie/Desktop/Virto Commerce/Content/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="114" documentId="10_ncr:100000_{F9F061A4-5A66-409B-95AF-88B363D95D8A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{466FEEAF-BF79-A547-8C5B-F249834A32FD}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9F6AF636-68E8-DE41-A539-3C1CDAD4E124}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" activeTab="7" xr2:uid="{0F76D96E-5F4C-C348-9B52-4890895C57F0}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" xr2:uid="{0F76D96E-5F4C-C348-9B52-4890895C57F0}"/>
   </bookViews>
   <sheets>
     <sheet name="How to Use" sheetId="1" r:id="rId1"/>
@@ -2480,18 +2480,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2512,6 +2500,18 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2552,30 +2552,22 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2587,6 +2579,12 @@
     <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2597,10 +2595,12 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2619,18 +2619,18 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3198,7 +3198,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D71FA74-3E83-7943-8A2F-CBA5CAE7A7B9}">
   <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
   <cols>
@@ -3434,10 +3434,10 @@
       <c r="D20" s="38">
         <v>10</v>
       </c>
-      <c r="E20" s="153" t="s">
+      <c r="E20" s="149" t="s">
         <v>248</v>
       </c>
-      <c r="F20" s="154"/>
+      <c r="F20" s="150"/>
       <c r="G20" s="3"/>
       <c r="H20" s="1"/>
     </row>
@@ -3450,10 +3450,10 @@
       <c r="D21" s="38">
         <v>5</v>
       </c>
-      <c r="E21" s="155" t="s">
+      <c r="E21" s="151" t="s">
         <v>5</v>
       </c>
-      <c r="F21" s="156"/>
+      <c r="F21" s="152"/>
       <c r="G21" s="3"/>
       <c r="H21" s="1"/>
     </row>
@@ -3466,10 +3466,10 @@
       <c r="D22" s="38">
         <v>0</v>
       </c>
-      <c r="E22" s="155" t="s">
+      <c r="E22" s="151" t="s">
         <v>253</v>
       </c>
-      <c r="F22" s="156"/>
+      <c r="F22" s="152"/>
       <c r="G22" s="3"/>
       <c r="H22" s="1"/>
     </row>
@@ -3482,10 +3482,10 @@
       <c r="D23" s="38">
         <v>0</v>
       </c>
-      <c r="E23" s="157" t="s">
+      <c r="E23" s="153" t="s">
         <v>8</v>
       </c>
-      <c r="F23" s="158"/>
+      <c r="F23" s="154"/>
       <c r="G23" s="3"/>
       <c r="H23" s="1"/>
     </row>
@@ -3498,10 +3498,10 @@
       <c r="D24" s="38">
         <v>0</v>
       </c>
-      <c r="E24" s="159" t="s">
+      <c r="E24" s="155" t="s">
         <v>10</v>
       </c>
-      <c r="F24" s="160"/>
+      <c r="F24" s="156"/>
       <c r="G24" s="3"/>
       <c r="H24" s="1"/>
     </row>
@@ -3509,8 +3509,8 @@
       <c r="A25" s="1"/>
       <c r="B25" s="3"/>
       <c r="C25" s="9"/>
-      <c r="D25" s="151"/>
-      <c r="E25" s="152"/>
+      <c r="D25" s="147"/>
+      <c r="E25" s="148"/>
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
       <c r="H25" s="1"/>
@@ -3521,11 +3521,11 @@
       <c r="C26" s="11" t="s">
         <v>232</v>
       </c>
-      <c r="D26" s="147" t="s">
+      <c r="D26" s="157" t="s">
         <v>3</v>
       </c>
-      <c r="E26" s="147"/>
-      <c r="F26" s="148"/>
+      <c r="E26" s="157"/>
+      <c r="F26" s="158"/>
       <c r="G26" s="3"/>
       <c r="H26" s="1"/>
     </row>
@@ -3535,11 +3535,11 @@
       <c r="C27" s="33" t="s">
         <v>235</v>
       </c>
-      <c r="D27" s="149" t="s">
+      <c r="D27" s="159" t="s">
         <v>239</v>
       </c>
-      <c r="E27" s="149"/>
-      <c r="F27" s="149"/>
+      <c r="E27" s="159"/>
+      <c r="F27" s="159"/>
       <c r="G27" s="3"/>
       <c r="H27" s="1"/>
     </row>
@@ -3549,11 +3549,11 @@
       <c r="C28" s="34" t="s">
         <v>236</v>
       </c>
-      <c r="D28" s="149" t="s">
+      <c r="D28" s="159" t="s">
         <v>241</v>
       </c>
-      <c r="E28" s="149"/>
-      <c r="F28" s="149"/>
+      <c r="E28" s="159"/>
+      <c r="F28" s="159"/>
       <c r="G28" s="3"/>
       <c r="H28" s="1"/>
     </row>
@@ -3563,11 +3563,11 @@
       <c r="C29" s="35" t="s">
         <v>237</v>
       </c>
-      <c r="D29" s="150" t="s">
+      <c r="D29" s="160" t="s">
         <v>242</v>
       </c>
-      <c r="E29" s="150"/>
-      <c r="F29" s="150"/>
+      <c r="E29" s="160"/>
+      <c r="F29" s="160"/>
       <c r="G29" s="3"/>
       <c r="H29" s="1"/>
     </row>
@@ -3577,11 +3577,11 @@
       <c r="C30" s="129" t="s">
         <v>238</v>
       </c>
-      <c r="D30" s="149" t="s">
+      <c r="D30" s="159" t="s">
         <v>240</v>
       </c>
-      <c r="E30" s="149"/>
-      <c r="F30" s="149"/>
+      <c r="E30" s="159"/>
+      <c r="F30" s="159"/>
       <c r="G30" s="3"/>
       <c r="H30" s="1"/>
     </row>
@@ -3615,11 +3615,11 @@
       <c r="C33" s="11" t="s">
         <v>243</v>
       </c>
-      <c r="D33" s="147" t="s">
+      <c r="D33" s="157" t="s">
         <v>3</v>
       </c>
-      <c r="E33" s="147"/>
-      <c r="F33" s="148"/>
+      <c r="E33" s="157"/>
+      <c r="F33" s="158"/>
       <c r="G33" s="3"/>
       <c r="H33" s="1"/>
     </row>
@@ -3629,11 +3629,11 @@
       <c r="C34" s="33" t="s">
         <v>244</v>
       </c>
-      <c r="D34" s="149" t="s">
+      <c r="D34" s="159" t="s">
         <v>246</v>
       </c>
-      <c r="E34" s="149"/>
-      <c r="F34" s="149"/>
+      <c r="E34" s="159"/>
+      <c r="F34" s="159"/>
       <c r="G34" s="3"/>
       <c r="H34" s="1"/>
     </row>
@@ -3643,11 +3643,11 @@
       <c r="C35" s="34" t="s">
         <v>245</v>
       </c>
-      <c r="D35" s="149" t="s">
+      <c r="D35" s="159" t="s">
         <v>247</v>
       </c>
-      <c r="E35" s="149"/>
-      <c r="F35" s="149"/>
+      <c r="E35" s="159"/>
+      <c r="F35" s="159"/>
       <c r="G35" s="3"/>
       <c r="H35" s="1"/>
     </row>
@@ -3713,12 +3713,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="E24:F24"/>
     <mergeCell ref="D26:F26"/>
     <mergeCell ref="D34:F34"/>
     <mergeCell ref="D35:F35"/>
@@ -3727,6 +3721,12 @@
     <mergeCell ref="D29:F29"/>
     <mergeCell ref="D30:F30"/>
     <mergeCell ref="D33:F33"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="E24:F24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5334,224 +5334,224 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="27"/>
-      <c r="B5" s="200" t="s">
+      <c r="B5" s="202" t="s">
         <v>15</v>
       </c>
       <c r="C5" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="204"/>
-      <c r="E5" s="205"/>
+      <c r="D5" s="183"/>
+      <c r="E5" s="184"/>
       <c r="F5" s="50"/>
       <c r="G5" s="27"/>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="27"/>
-      <c r="B6" s="197"/>
+      <c r="B6" s="199"/>
       <c r="C6" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="202"/>
-      <c r="E6" s="203"/>
+      <c r="D6" s="179"/>
+      <c r="E6" s="180"/>
       <c r="F6" s="51"/>
       <c r="G6" s="27"/>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="27"/>
-      <c r="B7" s="197"/>
+      <c r="B7" s="199"/>
       <c r="C7" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="202"/>
-      <c r="E7" s="203"/>
+      <c r="D7" s="179"/>
+      <c r="E7" s="180"/>
       <c r="F7" s="51"/>
       <c r="G7" s="27"/>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="27"/>
-      <c r="B8" s="197"/>
+      <c r="B8" s="199"/>
       <c r="C8" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="202"/>
-      <c r="E8" s="203"/>
+      <c r="D8" s="179"/>
+      <c r="E8" s="180"/>
       <c r="F8" s="51"/>
       <c r="G8" s="27"/>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="27"/>
-      <c r="B9" s="197"/>
+      <c r="B9" s="199"/>
       <c r="C9" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="202"/>
-      <c r="E9" s="203"/>
+      <c r="D9" s="179"/>
+      <c r="E9" s="180"/>
       <c r="F9" s="51"/>
       <c r="G9" s="27"/>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="27"/>
-      <c r="B10" s="197"/>
+      <c r="B10" s="199"/>
       <c r="C10" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="202"/>
-      <c r="E10" s="203"/>
+      <c r="D10" s="179"/>
+      <c r="E10" s="180"/>
       <c r="F10" s="51"/>
       <c r="G10" s="27"/>
     </row>
     <row r="11" spans="1:7" ht="17" thickBot="1">
       <c r="A11" s="27"/>
-      <c r="B11" s="201"/>
+      <c r="B11" s="203"/>
       <c r="C11" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="202"/>
-      <c r="E11" s="203"/>
+      <c r="D11" s="179"/>
+      <c r="E11" s="180"/>
       <c r="F11" s="59"/>
       <c r="G11" s="27"/>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="27"/>
-      <c r="B12" s="196" t="s">
+      <c r="B12" s="198" t="s">
         <v>23</v>
       </c>
       <c r="C12" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="D12" s="206"/>
-      <c r="E12" s="207"/>
+      <c r="D12" s="181"/>
+      <c r="E12" s="182"/>
       <c r="F12" s="53"/>
       <c r="G12" s="27"/>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="27"/>
-      <c r="B13" s="196"/>
+      <c r="B13" s="198"/>
       <c r="C13" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="D13" s="194"/>
-      <c r="E13" s="195"/>
+      <c r="D13" s="177"/>
+      <c r="E13" s="178"/>
       <c r="F13" s="54"/>
       <c r="G13" s="27"/>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="27"/>
-      <c r="B14" s="196"/>
+      <c r="B14" s="198"/>
       <c r="C14" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="D14" s="194"/>
-      <c r="E14" s="195"/>
+      <c r="D14" s="177"/>
+      <c r="E14" s="178"/>
       <c r="F14" s="54"/>
       <c r="G14" s="27"/>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="27"/>
-      <c r="B15" s="196"/>
+      <c r="B15" s="198"/>
       <c r="C15" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="D15" s="194"/>
-      <c r="E15" s="195"/>
+      <c r="D15" s="177"/>
+      <c r="E15" s="178"/>
       <c r="F15" s="54"/>
       <c r="G15" s="27"/>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="27"/>
-      <c r="B16" s="196"/>
+      <c r="B16" s="198"/>
       <c r="C16" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="D16" s="194"/>
-      <c r="E16" s="195"/>
+      <c r="D16" s="177"/>
+      <c r="E16" s="178"/>
       <c r="F16" s="54"/>
       <c r="G16" s="27"/>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="27"/>
-      <c r="B17" s="196"/>
+      <c r="B17" s="198"/>
       <c r="C17" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="D17" s="194"/>
-      <c r="E17" s="195"/>
+      <c r="D17" s="177"/>
+      <c r="E17" s="178"/>
       <c r="F17" s="54"/>
       <c r="G17" s="27"/>
     </row>
     <row r="18" spans="1:7" ht="17" thickBot="1">
       <c r="A18" s="27"/>
-      <c r="B18" s="196"/>
+      <c r="B18" s="198"/>
       <c r="C18" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="D18" s="194"/>
-      <c r="E18" s="195"/>
+      <c r="D18" s="177"/>
+      <c r="E18" s="178"/>
       <c r="F18" s="54"/>
       <c r="G18" s="27"/>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="27"/>
-      <c r="B19" s="197" t="s">
+      <c r="B19" s="199" t="s">
         <v>31</v>
       </c>
       <c r="C19" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="D19" s="181"/>
-      <c r="E19" s="182"/>
+      <c r="D19" s="196"/>
+      <c r="E19" s="197"/>
       <c r="F19" s="50"/>
       <c r="G19" s="27"/>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="27"/>
-      <c r="B20" s="197"/>
+      <c r="B20" s="199"/>
       <c r="C20" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="D20" s="183"/>
-      <c r="E20" s="184"/>
+      <c r="D20" s="190"/>
+      <c r="E20" s="191"/>
       <c r="F20" s="51"/>
       <c r="G20" s="27"/>
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="27"/>
-      <c r="B21" s="197"/>
+      <c r="B21" s="199"/>
       <c r="C21" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="D21" s="183"/>
-      <c r="E21" s="184"/>
+      <c r="D21" s="190"/>
+      <c r="E21" s="191"/>
       <c r="F21" s="51"/>
       <c r="G21" s="27"/>
     </row>
     <row r="22" spans="1:7" ht="17" thickBot="1">
       <c r="A22" s="27"/>
-      <c r="B22" s="197"/>
+      <c r="B22" s="199"/>
       <c r="C22" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="D22" s="190"/>
-      <c r="E22" s="191"/>
+      <c r="D22" s="192"/>
+      <c r="E22" s="193"/>
       <c r="F22" s="52"/>
       <c r="G22" s="27"/>
     </row>
     <row r="23" spans="1:7">
       <c r="A23" s="27"/>
-      <c r="B23" s="198" t="s">
+      <c r="B23" s="200" t="s">
         <v>36</v>
       </c>
       <c r="C23" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="D23" s="192"/>
-      <c r="E23" s="193"/>
+      <c r="D23" s="194"/>
+      <c r="E23" s="195"/>
       <c r="F23" s="53"/>
       <c r="G23" s="27"/>
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="27"/>
-      <c r="B24" s="196"/>
+      <c r="B24" s="198"/>
       <c r="C24" s="17" t="s">
         <v>38</v>
       </c>
@@ -5562,7 +5562,7 @@
     </row>
     <row r="25" spans="1:7">
       <c r="A25" s="27"/>
-      <c r="B25" s="196"/>
+      <c r="B25" s="198"/>
       <c r="C25" s="17" t="s">
         <v>39</v>
       </c>
@@ -5573,7 +5573,7 @@
     </row>
     <row r="26" spans="1:7">
       <c r="A26" s="27"/>
-      <c r="B26" s="196"/>
+      <c r="B26" s="198"/>
       <c r="C26" s="17" t="s">
         <v>40</v>
       </c>
@@ -5584,7 +5584,7 @@
     </row>
     <row r="27" spans="1:7" ht="17" thickBot="1">
       <c r="A27" s="27"/>
-      <c r="B27" s="199"/>
+      <c r="B27" s="201"/>
       <c r="C27" s="18" t="s">
         <v>41</v>
       </c>
@@ -5595,58 +5595,58 @@
     </row>
     <row r="28" spans="1:7">
       <c r="A28" s="27"/>
-      <c r="B28" s="179" t="s">
+      <c r="B28" s="206" t="s">
         <v>42</v>
       </c>
       <c r="C28" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="D28" s="181"/>
-      <c r="E28" s="182"/>
+      <c r="D28" s="196"/>
+      <c r="E28" s="197"/>
       <c r="F28" s="50"/>
       <c r="G28" s="27"/>
     </row>
     <row r="29" spans="1:7">
       <c r="A29" s="27"/>
-      <c r="B29" s="179"/>
+      <c r="B29" s="206"/>
       <c r="C29" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="D29" s="183"/>
-      <c r="E29" s="184"/>
+      <c r="D29" s="190"/>
+      <c r="E29" s="191"/>
       <c r="F29" s="51"/>
       <c r="G29" s="27"/>
     </row>
     <row r="30" spans="1:7">
       <c r="A30" s="27"/>
-      <c r="B30" s="179"/>
+      <c r="B30" s="206"/>
       <c r="C30" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="D30" s="183"/>
-      <c r="E30" s="184"/>
+      <c r="D30" s="190"/>
+      <c r="E30" s="191"/>
       <c r="F30" s="51"/>
       <c r="G30" s="27"/>
     </row>
     <row r="31" spans="1:7">
       <c r="A31" s="27"/>
-      <c r="B31" s="179"/>
+      <c r="B31" s="206"/>
       <c r="C31" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="D31" s="183"/>
-      <c r="E31" s="184"/>
+      <c r="D31" s="190"/>
+      <c r="E31" s="191"/>
       <c r="F31" s="51"/>
       <c r="G31" s="27"/>
     </row>
     <row r="32" spans="1:7" ht="17" thickBot="1">
       <c r="A32" s="27"/>
-      <c r="B32" s="180"/>
+      <c r="B32" s="207"/>
       <c r="C32" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="D32" s="177"/>
-      <c r="E32" s="178"/>
+      <c r="D32" s="204"/>
+      <c r="E32" s="205"/>
       <c r="F32" s="52"/>
       <c r="G32" s="27"/>
     </row>
@@ -5742,18 +5742,12 @@
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="B28:B32"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="D31:E31"/>
     <mergeCell ref="D26:E26"/>
     <mergeCell ref="D27:E27"/>
     <mergeCell ref="B2:E3"/>
@@ -5770,12 +5764,18 @@
     <mergeCell ref="B19:B22"/>
     <mergeCell ref="B23:B27"/>
     <mergeCell ref="B5:B11"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="B28:B32"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D15:E15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5842,19 +5842,19 @@
     </row>
     <row r="5" spans="1:6" ht="27" customHeight="1">
       <c r="A5" s="27"/>
-      <c r="B5" s="200" t="s">
+      <c r="B5" s="202" t="s">
         <v>160</v>
       </c>
       <c r="C5" s="20" t="s">
         <v>161</v>
       </c>
-      <c r="D5" s="204"/>
+      <c r="D5" s="183"/>
       <c r="E5" s="209"/>
       <c r="F5" s="27"/>
     </row>
     <row r="6" spans="1:6" ht="27" customHeight="1">
       <c r="A6" s="27"/>
-      <c r="B6" s="197"/>
+      <c r="B6" s="199"/>
       <c r="C6" s="47" t="s">
         <v>162</v>
       </c>
@@ -5864,17 +5864,17 @@
     </row>
     <row r="7" spans="1:6" ht="27" customHeight="1">
       <c r="A7" s="27"/>
-      <c r="B7" s="197"/>
+      <c r="B7" s="199"/>
       <c r="C7" s="21" t="s">
         <v>163</v>
       </c>
-      <c r="D7" s="202"/>
+      <c r="D7" s="179"/>
       <c r="E7" s="210"/>
       <c r="F7" s="27"/>
     </row>
     <row r="8" spans="1:6" ht="27" customHeight="1" thickBot="1">
       <c r="A8" s="27"/>
-      <c r="B8" s="201"/>
+      <c r="B8" s="203"/>
       <c r="C8" s="46" t="s">
         <v>159</v>
       </c>
@@ -5914,7 +5914,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D11E105-49B9-A242-A011-FC98BD751921}">
   <dimension ref="A1:P47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="7.6640625" defaultRowHeight="16"/>
   <cols>
@@ -6930,12 +6930,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100312548E0A32D1E4992A054B539B2C8B7" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2d26257b09f6ba1dadcdd974360e52f8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="860f2592-fddf-445c-beb2-67311d690a50" xmlns:ns3="a3316952-4225-4e08-88ee-91bddcbcb857" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="69983652eb9ee6a6eb72fbfde8acffb7" ns2:_="" ns3:_="">
     <xsd:import namespace="860f2592-fddf-445c-beb2-67311d690a50"/>
@@ -7138,6 +7132,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -7148,23 +7148,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{866CD4F5-8C72-446F-AB58-DE50C2278F8E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="860f2592-fddf-445c-beb2-67311d690a50"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="a3316952-4225-4e08-88ee-91bddcbcb857"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DBE7B7DF-EEE3-46ED-AF82-D5BB5ED08683}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7183,6 +7166,23 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{866CD4F5-8C72-446F-AB58-DE50C2278F8E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="860f2592-fddf-445c-beb2-67311d690a50"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="a3316952-4225-4e08-88ee-91bddcbcb857"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{93A57C36-18AD-40F2-A6DC-C48A57356F46}">
   <ds:schemaRefs>

</xml_diff>